<commit_message>
test with different params for AILabxTest2_3.py
</commit_message>
<xml_diff>
--- a/SRC/BackTest/data/AILabxTest2_3_info_2000_20250620.xlsx
+++ b/SRC/BackTest/data/AILabxTest2_3_info_2000_20250620.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>pnl_ratio</t>
   </si>
@@ -99,6 +99,1023 @@
   <si>
     <t>backtest_marginfloat_ratio2=0.4,</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>index_list = {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF7A7E85"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t># List</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF7A7E85"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SZSE.159509"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>纳指科技</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.518880"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>黄金</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.512480"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>半导体</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SZSE.159531"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中证</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2000ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.513100"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>纳指</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.513520"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>日经</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SZSE.159857"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>光伏</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.512100"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>中证</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1000ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.510180"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>上证</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>180ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.588000"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>科创</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>50ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.513330"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>恒生互联网</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SZSE.162719"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>石油</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>LOF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.513500"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>标普</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>500ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SZSE.159915"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>创业板</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"SHSE.513030"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>德国</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FF6AAB73"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ETF"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.8"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -110,7 +1127,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +1143,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9.8"/>
       <name val="Courier New"/>
       <charset val="134"/>
@@ -140,6 +1150,18 @@
     <font>
       <sz val="9.8"/>
       <color rgb="FF7A7E85"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.8"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.8"/>
+      <color rgb="FF6AAB73"/>
       <name val="Courier New"/>
       <charset val="134"/>
     </font>
@@ -286,6 +1308,12 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8"/>
+      <color rgb="FF6AAB73"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -606,31 +1634,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -639,127 +1664,132 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1109,7 +2139,7 @@
   <dimension ref="A1:J2001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J17" sqref="J17:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1228,7 +2258,7 @@
       <c r="H4">
         <v>0.2</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
@@ -1255,7 +2285,7 @@
       <c r="H5">
         <v>0.2</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1284,7 +2314,7 @@
       <c r="H6">
         <v>0.2</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1313,7 +2343,7 @@
       <c r="H7">
         <v>0.22</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1342,7 +2372,7 @@
       <c r="H8">
         <v>0.23</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1371,7 +2401,7 @@
       <c r="H9">
         <v>0.21</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1400,7 +2430,7 @@
       <c r="H10">
         <v>0.2</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1429,7 +2459,7 @@
       <c r="H11">
         <v>0.2</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1458,7 +2488,7 @@
       <c r="H12">
         <v>0.2</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1487,7 +2517,7 @@
       <c r="H13">
         <v>0.2</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1516,7 +2546,7 @@
       <c r="H14">
         <v>0.22</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1572,7 +2602,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>5.02528132134896</v>
       </c>
@@ -1597,8 +2627,11 @@
       <c r="H17">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="J17" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>5.0121852023149</v>
       </c>
@@ -1623,8 +2656,11 @@
       <c r="H18">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="J18" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>4.97619847812181</v>
       </c>
@@ -1649,8 +2685,11 @@
       <c r="H19">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="J19" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>4.97572254869401</v>
       </c>
@@ -1675,8 +2714,11 @@
       <c r="H20">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="J20" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>4.96650338094004</v>
       </c>
@@ -1701,8 +2743,11 @@
       <c r="H21">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="J21" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>4.96076142797475</v>
       </c>
@@ -1727,8 +2772,11 @@
       <c r="H22">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="J22" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>4.95219012992766</v>
       </c>
@@ -1753,8 +2801,11 @@
       <c r="H23">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="J23" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>4.95177872101606</v>
       </c>
@@ -1779,8 +2830,11 @@
       <c r="H24">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="J24" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>4.95174113315648</v>
       </c>
@@ -1805,8 +2859,11 @@
       <c r="H25">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="J25" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>4.95137982648775</v>
       </c>
@@ -1831,8 +2888,11 @@
       <c r="H26">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="J26" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>4.94761767414559</v>
       </c>
@@ -1857,8 +2917,11 @@
       <c r="H27">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="J27" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>4.94648487762381</v>
       </c>
@@ -1883,8 +2946,11 @@
       <c r="H28">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="J28" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>4.94594405715644</v>
       </c>
@@ -1909,8 +2975,11 @@
       <c r="H29">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="J29" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>4.93898767210894</v>
       </c>
@@ -1935,8 +3004,11 @@
       <c r="H30">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="J30" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>4.92849209671362</v>
       </c>
@@ -1961,8 +3033,11 @@
       <c r="H31">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="J31" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>4.92705100049387</v>
       </c>
@@ -1987,8 +3062,11 @@
       <c r="H32">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="J32" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>4.92611966388485</v>
       </c>
@@ -2012,6 +3090,9 @@
       </c>
       <c r="H33">
         <v>0.23</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2040,7 +3121,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>4.90803167066434</v>
       </c>
@@ -2064,6 +3145,9 @@
       </c>
       <c r="H35">
         <v>0.23</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -53184,7 +54268,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H2001">
-    <sortState ref="A2:H2001">
+    <sortState ref="A1:H2001">
       <sortCondition ref="A1" descending="1"/>
     </sortState>
     <extLst/>

</xml_diff>